<commit_message>
Added read excel data changes and put additional time holds
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/AutomationTest-1.xlsx
+++ b/src/test/java/Resources/AutomationTest-1.xlsx
@@ -620,7 +620,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -755,7 +757,7 @@
         <v>64171</v>
       </c>
       <c r="S2" s="17">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="T2" s="9">
         <v>1.3022100000000001</v>
@@ -818,9 +820,11 @@
       <c r="Q3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="21"/>
+      <c r="R3" s="17">
+        <v>64171</v>
+      </c>
       <c r="S3" s="25">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="T3" s="19">
         <v>0.3024</v>
@@ -883,9 +887,11 @@
       <c r="Q4" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="21"/>
+      <c r="R4" s="17">
+        <v>64171</v>
+      </c>
       <c r="S4" s="25">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="T4" s="19">
         <v>0.6</v>
@@ -952,7 +958,7 @@
         <v>73042</v>
       </c>
       <c r="S5" s="17">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="T5" s="19">
         <v>0.52439999999999998</v>
@@ -1015,9 +1021,11 @@
       <c r="Q6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="21"/>
+      <c r="R6" s="25">
+        <v>73042</v>
+      </c>
       <c r="S6" s="25">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="T6" s="19">
         <v>0.60287999999999997</v>
@@ -1080,9 +1088,11 @@
       <c r="Q7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R7" s="21"/>
-      <c r="S7" s="17">
-        <v>17</v>
+      <c r="R7" s="25">
+        <v>73042</v>
+      </c>
+      <c r="S7" s="25">
+        <v>20</v>
       </c>
       <c r="T7" s="19">
         <v>0.80262</v>
@@ -1145,9 +1155,11 @@
       <c r="Q8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R8" s="21"/>
-      <c r="S8" s="25">
-        <v>18</v>
+      <c r="R8" s="25">
+        <v>73042</v>
+      </c>
+      <c r="S8" s="17">
+        <v>21</v>
       </c>
       <c r="T8" s="19">
         <v>0.14112</v>
@@ -1210,9 +1222,11 @@
       <c r="Q9" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="21"/>
+      <c r="R9" s="25">
+        <v>73042</v>
+      </c>
       <c r="S9" s="25">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="T9" s="19">
         <v>5.9400000000000001E-2</v>
@@ -1275,9 +1289,11 @@
       <c r="Q10" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="21"/>
-      <c r="S10" s="17">
-        <v>20</v>
+      <c r="R10" s="25">
+        <v>73042</v>
+      </c>
+      <c r="S10" s="25">
+        <v>23</v>
       </c>
       <c r="T10" s="19">
         <v>0.36480000000000001</v>
@@ -1343,8 +1359,8 @@
       <c r="R11" s="25">
         <v>1751</v>
       </c>
-      <c r="S11" s="25">
-        <v>21</v>
+      <c r="S11" s="17">
+        <v>24</v>
       </c>
       <c r="T11" s="19">
         <v>5.9400000000000001E-2</v>

</xml_diff>